<commit_message>
99.23% accuracy and faster
</commit_message>
<xml_diff>
--- a/data/OFFICIAL-TEST-SET-1.xlsx
+++ b/data/OFFICIAL-TEST-SET-1.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="157" documentId="11_79DA2B6B5C3787F24A9A54D881E28314B5F12F84" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FFACFD7-B3A7-46D2-89E4-89C5F60E826F}"/>
   <bookViews>
-    <workbookView xWindow="855" yWindow="5610" windowWidth="18900" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3675" yWindow="0" windowWidth="15885" windowHeight="9900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WS-Data" sheetId="1" r:id="rId1"/>
@@ -1192,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BN16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="H4" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>